<commit_message>
Daily 04.07 took place
</commit_message>
<xml_diff>
--- a/challenge_4/SCRUM/Daily Documentation.xlsx
+++ b/challenge_4/SCRUM/Daily Documentation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tom" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -46,6 +46,15 @@
     <t xml:space="preserve">network connection problems at the ITECH</t>
   </si>
   <si>
+    <t xml:space="preserve">starting with the website </t>
+  </si>
+  <si>
+    <t xml:space="preserve">working on the website </t>
+  </si>
+  <si>
+    <t xml:space="preserve">limited knwoledge</t>
+  </si>
+  <si>
     <t xml:space="preserve">playing FIFA</t>
   </si>
   <si>
@@ -55,6 +64,15 @@
     <t xml:space="preserve">i am tired of my life (jk)</t>
   </si>
   <si>
+    <t xml:space="preserve">scrum organisation, helping Raik with the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database, hopefully starting with the hardware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sql syntax</t>
+  </si>
+  <si>
     <t xml:space="preserve">chilling my life</t>
   </si>
   <si>
@@ -64,6 +82,15 @@
     <t xml:space="preserve">nothing, i am the fkn best</t>
   </si>
   <si>
+    <t xml:space="preserve">database, erm and dump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">working on the sql dump, hardware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sql syntax of course</t>
+  </si>
+  <si>
     <t xml:space="preserve">enjoying the weekend</t>
   </si>
   <si>
@@ -71,6 +98,15 @@
   </si>
   <si>
     <t xml:space="preserve">my illness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">starting with the website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VM problems solving, Linux things</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linux</t>
   </si>
 </sst>
 </file>
@@ -183,8 +219,8 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -225,6 +261,15 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>45111</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,14 +321,14 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,70 +350,58 @@
         <v>45110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>45111</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>45112</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>45113</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>45114</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>45117</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>45118</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>45119</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -388,15 +421,15 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -418,70 +451,58 @@
         <v>45110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>45111</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>45112</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>45113</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>45114</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>45117</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>45118</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>45119</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -502,14 +523,14 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -531,70 +552,58 @@
         <v>45110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>45111</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>45112</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>45113</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>45114</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>45117</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>45118</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>45119</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>